<commit_message>
added chart of chronic users
</commit_message>
<xml_diff>
--- a/2-heroin/h.xlsx
+++ b/2-heroin/h.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24220" yWindow="0" windowWidth="14100" windowHeight="21140" tabRatio="660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29460" windowHeight="21140" tabRatio="660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="5" r:id="rId1"/>
@@ -2958,7 +2958,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="134">
+  <cellStyleXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3043,6 +3043,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3190,7 +3200,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="134">
+  <cellStyles count="144">
     <cellStyle name="Comma 2" xfId="46"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3257,6 +3267,11 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3322,6 +3337,11 @@
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="45"/>
     <cellStyle name="Percent" xfId="83" builtinId="5"/>
@@ -3727,10 +3747,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C16" sqref="A1:C16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3738,7 +3758,7 @@
     <col min="1" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -3749,7 +3769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:3">
       <c r="A2" s="45">
         <v>1999</v>
       </c>
@@ -3759,16 +3779,8 @@
       <c r="C2" s="8">
         <v>1654</v>
       </c>
-      <c r="E2" s="8">
-        <f>-1</f>
-        <v>-1</v>
-      </c>
-      <c r="F2" s="8">
-        <f t="shared" ref="F2:F16" si="0">-1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="45">
         <v>2000</v>
       </c>
@@ -3778,16 +3790,8 @@
       <c r="C3" s="8">
         <v>1563</v>
       </c>
-      <c r="E3" s="8">
-        <f t="shared" ref="E3:F16" si="1">-1</f>
-        <v>-1</v>
-      </c>
-      <c r="F3" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="45">
         <v>2001</v>
       </c>
@@ -3797,16 +3801,8 @@
       <c r="C4" s="8">
         <v>1466</v>
       </c>
-      <c r="E4" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="45">
         <v>2002</v>
       </c>
@@ -3816,16 +3812,8 @@
       <c r="C5" s="8">
         <v>1730</v>
       </c>
-      <c r="E5" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F5" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="45">
         <v>2003</v>
       </c>
@@ -3835,16 +3823,8 @@
       <c r="C6" s="8">
         <v>1722</v>
       </c>
-      <c r="E6" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="45">
         <v>2004</v>
       </c>
@@ -3854,16 +3834,8 @@
       <c r="C7" s="8">
         <v>1537</v>
       </c>
-      <c r="E7" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F7" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="45">
         <v>2005</v>
       </c>
@@ -3873,16 +3845,8 @@
       <c r="C8" s="8">
         <v>1620</v>
       </c>
-      <c r="E8" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="45">
         <v>2006</v>
       </c>
@@ -3892,16 +3856,8 @@
       <c r="C9" s="8">
         <v>1744</v>
       </c>
-      <c r="E9" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F9" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="45">
         <v>2007</v>
       </c>
@@ -3911,16 +3867,8 @@
       <c r="C10" s="8">
         <v>2000</v>
       </c>
-      <c r="E10" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="45">
         <v>2008</v>
       </c>
@@ -3930,16 +3878,8 @@
       <c r="C11" s="8">
         <v>2490</v>
       </c>
-      <c r="E11" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F11" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="45">
         <v>2009</v>
       </c>
@@ -3949,16 +3889,8 @@
       <c r="C12" s="8">
         <v>2701</v>
       </c>
-      <c r="E12" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F12" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="45">
         <v>2010</v>
       </c>
@@ -3968,16 +3900,8 @@
       <c r="C13" s="8">
         <v>2452</v>
       </c>
-      <c r="E13" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F13" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="45">
         <v>2011</v>
       </c>
@@ -3987,16 +3911,8 @@
       <c r="C14" s="8">
         <v>3519</v>
       </c>
-      <c r="E14" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="45">
         <v>2012</v>
       </c>
@@ -4006,16 +3922,8 @@
       <c r="C15" s="8">
         <v>4712</v>
       </c>
-      <c r="E15" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F15" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="45">
         <v>2013</v>
       </c>
@@ -4024,14 +3932,6 @@
       </c>
       <c r="C16" s="8">
         <v>6525</v>
-      </c>
-      <c r="E16" s="8">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="F16" s="8">
-        <f t="shared" si="0"/>
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -5539,8 +5439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5561,10 +5461,10 @@
         <v>2000</v>
       </c>
       <c r="B2" s="43">
-        <v>170</v>
+        <v>170000</v>
       </c>
       <c r="C2" s="43">
-        <v>1400</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5572,10 +5472,10 @@
         <v>2001</v>
       </c>
       <c r="B3" s="43">
-        <v>130</v>
+        <v>130000</v>
       </c>
       <c r="C3" s="43">
-        <v>1400</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5583,10 +5483,10 @@
         <v>2002</v>
       </c>
       <c r="B4" s="43">
-        <v>210</v>
+        <v>210000</v>
       </c>
       <c r="C4" s="43">
-        <v>1300</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5594,10 +5494,10 @@
         <v>2003</v>
       </c>
       <c r="B5" s="43">
-        <v>130</v>
+        <v>130000</v>
       </c>
       <c r="C5" s="43">
-        <v>1300</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5605,10 +5505,10 @@
         <v>2004</v>
       </c>
       <c r="B6" s="43">
-        <v>120</v>
+        <v>120000</v>
       </c>
       <c r="C6" s="43">
-        <v>1300</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5616,10 +5516,10 @@
         <v>2005</v>
       </c>
       <c r="B7" s="43">
-        <v>180</v>
+        <v>180000</v>
       </c>
       <c r="C7" s="43">
-        <v>1200</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5627,10 +5527,10 @@
         <v>2006</v>
       </c>
       <c r="B8" s="43">
-        <v>380</v>
+        <v>380000</v>
       </c>
       <c r="C8" s="43">
-        <v>1200</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5638,10 +5538,10 @@
         <v>2007</v>
       </c>
       <c r="B9" s="43">
-        <v>150</v>
+        <v>150000</v>
       </c>
       <c r="C9" s="43">
-        <v>1200</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5649,10 +5549,10 @@
         <v>2008</v>
       </c>
       <c r="B10" s="43">
-        <v>240</v>
+        <v>240000</v>
       </c>
       <c r="C10" s="43">
-        <v>1300</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5660,10 +5560,10 @@
         <v>2009</v>
       </c>
       <c r="B11" s="43">
-        <v>340</v>
+        <v>340000</v>
       </c>
       <c r="C11" s="43">
-        <v>1500</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5671,10 +5571,10 @@
         <v>2010</v>
       </c>
       <c r="B12" s="43">
-        <v>330</v>
+        <v>330000</v>
       </c>
       <c r="C12" s="43">
-        <v>1500</v>
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>